<commit_message>
Merged PR 138: updated excel with Test1 env information
updated excel with Test1 env information

Related work items: #4492
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
+++ b/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\Icon\DevOps\Server Setup\Security\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpesh.patel\source\repos\SCAD\DevOps\Server Setup\Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC302FBE-0897-4F4B-83AE-D784722A78F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server List" sheetId="4" r:id="rId1"/>
@@ -17,6 +18,10 @@
     <sheet name="Folder Perms" sheetId="2" r:id="rId3"/>
     <sheet name="Perms Reference" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Security Groups'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Server List'!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="106">
   <si>
     <t>WFM\Icon.Deploy.NonProd</t>
   </si>
@@ -286,12 +291,72 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>IRMATest1Job01</t>
+  </si>
+  <si>
+    <t>IRMATest1Job02</t>
+  </si>
+  <si>
+    <t>IRMATest1Job03</t>
+  </si>
+  <si>
+    <t>IRMATest1Job04</t>
+  </si>
+  <si>
+    <t>IRMATest1Job05</t>
+  </si>
+  <si>
+    <t>IRMATest1Job06</t>
+  </si>
+  <si>
+    <t>IRMATest1ETL01</t>
+  </si>
+  <si>
+    <t>IRMATest1Tidal01</t>
+  </si>
+  <si>
+    <t>IRMATest1Web01</t>
+  </si>
+  <si>
+    <t>IRMATest1Web02</t>
+  </si>
+  <si>
+    <t>IRMATest1Web03</t>
+  </si>
+  <si>
+    <t>IRMATest1Web04</t>
+  </si>
+  <si>
+    <t>IRMATest1Web05</t>
+  </si>
+  <si>
+    <t>IRMATest1Web06</t>
+  </si>
+  <si>
+    <t>WFM\IconInterfaceUserTes</t>
+  </si>
+  <si>
+    <t>wfm\MammothTest</t>
+  </si>
+  <si>
+    <t>wfm\IconWebTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,272 +704,624 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
         <v>65</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
         <v>67</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>70</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{41B0270A-C752-4B0D-A2E5-718FD9F44BE9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{39B8B737-EE3A-4067-9AAE-DB58AF03CE09}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -994,7 +1411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Merged PR 183: Updated Test1 user-security list.
Updated Test1 user-security list.

Related work items: #4490
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
+++ b/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpesh.patel\source\repos\SCAD\DevOps\Server Setup\Security\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Server Setup\Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC302FBE-0897-4F4B-83AE-D784722A78F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server List" sheetId="4" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Perms Reference" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Security Groups'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Security Groups'!$A$1:$E$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Server List'!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
   <si>
     <t>WFM\Icon.Deploy.NonProd</t>
   </si>
@@ -351,12 +350,21 @@
   </si>
   <si>
     <t>wfm\IconWebTest</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>only spore users are 'SPOReportsDev' and 'SPOReports'</t>
+  </si>
+  <si>
+    <t>WFM\NutriconServiceTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -704,7 +712,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -971,18 +979,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{41B0270A-C752-4B0D-A2E5-718FD9F44BE9}"/>
+  <autoFilter ref="A1:C1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,9 +998,10 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" customWidth="1"/>
     <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -1005,8 +1014,11 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1020,7 +1032,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1062,7 +1074,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1076,7 +1088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1090,7 +1102,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1118,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1146,7 +1158,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -1160,7 +1172,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1173,8 +1185,11 @@
       <c r="D13" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1188,7 +1203,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -1202,7 +1217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -1277,10 +1292,10 @@
         <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>66</v>
@@ -1291,10 +1306,10 @@
         <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
         <v>66</v>
@@ -1308,20 +1323,76 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D27" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{39B8B737-EE3A-4067-9AAE-DB58AF03CE09}"/>
+  <autoFilter ref="A1:E27"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1411,7 +1482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Merged PR 1392: IRMA Client QA1 configs and misc server-setup updates
- DataMonkey folders
- Created DVO and IRMA-log folder entries in security Excel file, with regional entries.
- added QA1 information
- Initial QA1 IRMA-Client config files with correct GUIDs and log path.
- Added explicity create for e:\webapps\ folder, so it's more clear.
- Encrypted the 2 conn strings in FL QA1 IRMA Client config.
- Renaming TSV input files to be generic (no env ref): the input-value spreadsheet will have values for all envs, so we don't need to save separate TSV files for each env; IIS script updated accordingly.
- For remaining 11 regions: encrypted the two connection strings for QA1 IRMA-Client config.  Plus format update for FL.
- Added loop for creating server-up file across list of web servers.

Related work items: #24930
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
+++ b/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Server List" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="147">
   <si>
     <t>WFM\Icon.Deploy.NonProd</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>Inherit (y or n)</t>
-  </si>
-  <si>
-    <t>E:\WebApps</t>
   </si>
   <si>
     <t>Perms (comma-delim, 
@@ -359,19 +356,143 @@
   </si>
   <si>
     <t>WFM\NutriconServiceTest</t>
+  </si>
+  <si>
+    <t>E:\Data\</t>
+  </si>
+  <si>
+    <t>E:\Data\DVO_Orders\</t>
+  </si>
+  <si>
+    <t>E:\</t>
+  </si>
+  <si>
+    <t>WFM\IRMATidalDev</t>
+  </si>
+  <si>
+    <t>E:\IRMA\</t>
+  </si>
+  <si>
+    <t>E:\IRMA\Logs\</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>Region Ref
+(don’t copy this column)</t>
+  </si>
+  <si>
+    <t>QA1</t>
+  </si>
+  <si>
+    <t>IRMAQAJob01</t>
+  </si>
+  <si>
+    <t>IRMAQAJob02</t>
+  </si>
+  <si>
+    <t>IRMAQAJob03</t>
+  </si>
+  <si>
+    <t>IRMAQAJob04</t>
+  </si>
+  <si>
+    <t>IRMAQAJob05</t>
+  </si>
+  <si>
+    <t>IRMAQAJob06</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb01</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb02</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb03</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb04</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb05</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb06</t>
+  </si>
+  <si>
+    <t>IRMAQAETL01</t>
+  </si>
+  <si>
+    <t>IRMAQATidal01</t>
+  </si>
+  <si>
+    <t>wfm\IconInterfaceUserQA</t>
+  </si>
+  <si>
+    <t>wfm\MammothQA</t>
+  </si>
+  <si>
+    <t>wfm\IconWebQA</t>
+  </si>
+  <si>
+    <t>WFM\NutriconServiceQA</t>
+  </si>
+  <si>
+    <t>E:\WebApps\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,10 +515,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -713,269 +838,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
+        <v>67</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" t="s">
-        <v>95</v>
+        <v>67</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s">
-        <v>90</v>
+        <v>64</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" t="s">
-        <v>91</v>
+        <v>64</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" t="s">
-        <v>92</v>
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>94</v>
+        <v>64</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>96</v>
+        <v>66</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>97</v>
+        <v>65</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" t="s">
-        <v>98</v>
+        <v>65</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>100</v>
+        <v>65</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" t="s">
-        <v>101</v>
+        <v>65</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>102</v>
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -987,10 +1266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -1015,26 +1294,26 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1043,12 +1322,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -1057,12 +1336,12 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1071,12 +1350,12 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1085,12 +1364,12 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1099,12 +1378,12 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1113,26 +1392,26 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1141,12 +1420,12 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1155,12 +1434,12 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1169,29 +1448,29 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1200,26 +1479,26 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -1228,12 +1507,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -1242,138 +1521,138 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1382,7 +1661,189 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1393,61 +1854,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A2:E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1456,24 +1919,1638 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" t="s">
-        <v>62</v>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F11, "\")</f>
+        <v>E:\Data\DVO_Orders\FL\</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F12, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\FL\Backup\</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F13, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\FL\Errors\</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F14, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\FL\Processing\</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F15, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\FL\Processing\Temp\</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F16, "\")</f>
+        <v>E:\IRMA\Logs\FL\</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F17, "\")</f>
+        <v>E:\Data\DVO_Orders\MA\</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F18, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\MA\Backup\</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F19, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\MA\Errors\</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F20, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\MA\Processing\</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F21, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\MA\Processing\Temp\</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F22, "\")</f>
+        <v>E:\IRMA\Logs\MA\</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F23, "\")</f>
+        <v>E:\Data\DVO_Orders\MW\</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F24, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\MW\Backup\</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F25, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\MW\Errors\</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F26, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\MW\Processing\</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F27, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\MW\Processing\Temp\</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F28, "\")</f>
+        <v>E:\IRMA\Logs\MW\</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F29, "\")</f>
+        <v>E:\Data\DVO_Orders\NA\</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F30, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\NA\Backup\</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F31, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\NA\Errors\</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F32, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\NA\Processing\</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F33, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\NA\Processing\Temp\</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F34, "\")</f>
+        <v>E:\IRMA\Logs\NA\</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F35, "\")</f>
+        <v>E:\Data\DVO_Orders\NC\</v>
+      </c>
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F36, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\NC\Backup\</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F37, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\NC\Errors\</v>
+      </c>
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F38, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\NC\Processing\</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F39, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\NC\Processing\Temp\</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F40, "\")</f>
+        <v>E:\IRMA\Logs\NC\</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" t="s">
+        <v>61</v>
+      </c>
+      <c r="F40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F41, "\")</f>
+        <v>E:\Data\DVO_Orders\NE\</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F42, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\NE\Backup\</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F43, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\NE\Errors\</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F44, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\NE\Processing\</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F45, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\NE\Processing\Temp\</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F46, "\")</f>
+        <v>E:\IRMA\Logs\NE\</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" t="s">
+        <v>61</v>
+      </c>
+      <c r="F46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F47, "\")</f>
+        <v>E:\Data\DVO_Orders\PN\</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F48, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\PN\Backup\</v>
+      </c>
+      <c r="C48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F49, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\PN\Errors\</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F50, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\PN\Processing\</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F51, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\PN\Processing\Temp\</v>
+      </c>
+      <c r="C51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F52, "\")</f>
+        <v>E:\IRMA\Logs\PN\</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" t="s">
+        <v>61</v>
+      </c>
+      <c r="F52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F53, "\")</f>
+        <v>E:\Data\DVO_Orders\RM\</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F54, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\RM\Backup\</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" t="s">
+        <v>80</v>
+      </c>
+      <c r="E54" t="s">
+        <v>61</v>
+      </c>
+      <c r="F54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F55, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\RM\Errors\</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" t="s">
+        <v>61</v>
+      </c>
+      <c r="F55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F56, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\RM\Processing\</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F57, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\RM\Processing\Temp\</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F58, "\")</f>
+        <v>E:\IRMA\Logs\RM\</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F59, "\")</f>
+        <v>E:\Data\DVO_Orders\SO\</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" t="s">
+        <v>61</v>
+      </c>
+      <c r="F59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F60, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\SO\Backup\</v>
+      </c>
+      <c r="C60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F61, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\SO\Errors\</v>
+      </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" t="s">
+        <v>61</v>
+      </c>
+      <c r="F61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F62, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\SO\Processing\</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" t="s">
+        <v>61</v>
+      </c>
+      <c r="F62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F63, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\SO\Processing\Temp\</v>
+      </c>
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="E63" t="s">
+        <v>61</v>
+      </c>
+      <c r="F63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F64, "\")</f>
+        <v>E:\IRMA\Logs\SO\</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="E64" t="s">
+        <v>61</v>
+      </c>
+      <c r="F64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F65, "\")</f>
+        <v>E:\Data\DVO_Orders\SP\</v>
+      </c>
+      <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" t="s">
+        <v>61</v>
+      </c>
+      <c r="F65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F66, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\SP\Backup\</v>
+      </c>
+      <c r="C66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" t="s">
+        <v>80</v>
+      </c>
+      <c r="E66" t="s">
+        <v>61</v>
+      </c>
+      <c r="F66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F67, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\SP\Errors\</v>
+      </c>
+      <c r="C67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" t="s">
+        <v>80</v>
+      </c>
+      <c r="E67" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F68, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\SP\Processing\</v>
+      </c>
+      <c r="C68" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F69, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\SP\Processing\Temp\</v>
+      </c>
+      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F69" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F70, "\")</f>
+        <v>E:\IRMA\Logs\SP\</v>
+      </c>
+      <c r="C70" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F71, "\")</f>
+        <v>E:\Data\DVO_Orders\SW\</v>
+      </c>
+      <c r="C71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" t="s">
+        <v>80</v>
+      </c>
+      <c r="E71" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F72, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\SW\Backup\</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F73, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\SW\Errors\</v>
+      </c>
+      <c r="C73" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" t="s">
+        <v>80</v>
+      </c>
+      <c r="E73" t="s">
+        <v>61</v>
+      </c>
+      <c r="F73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F74, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\SW\Processing\</v>
+      </c>
+      <c r="C74" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" t="s">
+        <v>80</v>
+      </c>
+      <c r="E74" t="s">
+        <v>61</v>
+      </c>
+      <c r="F74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F75, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\SW\Processing\Temp\</v>
+      </c>
+      <c r="C75" t="s">
+        <v>84</v>
+      </c>
+      <c r="D75" t="s">
+        <v>80</v>
+      </c>
+      <c r="E75" t="s">
+        <v>61</v>
+      </c>
+      <c r="F75" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F76, "\")</f>
+        <v>E:\IRMA\Logs\SW\</v>
+      </c>
+      <c r="C76" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" t="s">
+        <v>80</v>
+      </c>
+      <c r="E76" t="s">
+        <v>61</v>
+      </c>
+      <c r="F76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F77, "\")</f>
+        <v>E:\Data\DVO_Orders\UK\</v>
+      </c>
+      <c r="C77" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" t="s">
+        <v>80</v>
+      </c>
+      <c r="E77" t="s">
+        <v>61</v>
+      </c>
+      <c r="F77" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F78, "\Backup\")</f>
+        <v>E:\Data\DVO_Orders\UK\Backup\</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>80</v>
+      </c>
+      <c r="E78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F78" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F79, "\Errors\")</f>
+        <v>E:\Data\DVO_Orders\UK\Errors\</v>
+      </c>
+      <c r="C79" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" t="s">
+        <v>61</v>
+      </c>
+      <c r="F79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F80, "\Processing\")</f>
+        <v>E:\Data\DVO_Orders\UK\Processing\</v>
+      </c>
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" t="s">
+        <v>80</v>
+      </c>
+      <c r="E80" t="s">
+        <v>61</v>
+      </c>
+      <c r="F80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" t="str">
+        <f>_xlfn.CONCAT("E:\Data\DVO_Orders\", F81, "\Processing\Temp\")</f>
+        <v>E:\Data\DVO_Orders\UK\Processing\Temp\</v>
+      </c>
+      <c r="C81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" t="s">
+        <v>80</v>
+      </c>
+      <c r="E81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="str">
+        <f>_xlfn.CONCAT("E:\IRMA\Logs\", F82, "\")</f>
+        <v>E:\IRMA\Logs\UK\</v>
+      </c>
+      <c r="C82" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" t="s">
+        <v>80</v>
+      </c>
+      <c r="E82" t="s">
+        <v>61</v>
+      </c>
+      <c r="F82" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1686,10 +3763,10 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 1752: updated security script input excel with Perf, PROD, QA details
updated security script input excel with Perf, Prod, QA details
added VIM extract user

Related work items: #26576
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
+++ b/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Server Setup\Security\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpesh.patel\source\repos\SCAD\DevOps\Server Setup\Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B88C8EBA-2D50-40B5-9E53-05AB4DF9199C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server List" sheetId="4" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Security Groups'!$A$1:$E$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Server List'!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="207">
   <si>
     <t>WFM\Icon.Deploy.NonProd</t>
   </si>
@@ -474,12 +475,192 @@
   </si>
   <si>
     <t>E:\WebApps\</t>
+  </si>
+  <si>
+    <t>Etl</t>
+  </si>
+  <si>
+    <t>WFM\VIMExtractQA</t>
+  </si>
+  <si>
+    <t>WFM\VIMExtractTest</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>WFM\VIMExtractPrd</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb07</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb08</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb09</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb10</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb11</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb12</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb01</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb02</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb03</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb04</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb05</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfWeb06</t>
+  </si>
+  <si>
+    <t>Perf1</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob06</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob07</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob08</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob09</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob10</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob01</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob02</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob03</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob04</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfJob05</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfETL02</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfETL01</t>
+  </si>
+  <si>
+    <t>TIDAL</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfTidal02</t>
+  </si>
+  <si>
+    <t>IRMAQA-PerfTidal01</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb01</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb07</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb02</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb08</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb03</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb09</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb04</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb10</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb05</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb11</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb06</t>
+  </si>
+  <si>
+    <t>IRMAPrdWeb12</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob01</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob06</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob02</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob07</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob03</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob08</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob04</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob09</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob5</t>
+  </si>
+  <si>
+    <t>IRMAPrdJob10</t>
+  </si>
+  <si>
+    <t>IRMAPrdETL02</t>
+  </si>
+  <si>
+    <t>IRMAPrdETL01</t>
+  </si>
+  <si>
+    <t>IRMAPrdTidal01</t>
+  </si>
+  <si>
+    <t>IRMAPrdTidal02</t>
+  </si>
+  <si>
+    <t>PROD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -523,6 +704,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,11 +1021,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1426,7 @@
       <c r="B36" t="s">
         <v>67</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1253,23 +1437,595 @@
       <c r="B37" t="s">
         <v>66</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>141</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>164</v>
+      </c>
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>164</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>177</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>164</v>
+      </c>
+      <c r="B63" t="s">
+        <v>177</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>206</v>
+      </c>
+      <c r="B65" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>206</v>
+      </c>
+      <c r="B69" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" t="s">
+        <v>65</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>206</v>
+      </c>
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>206</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>206</v>
+      </c>
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>206</v>
+      </c>
+      <c r="B83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>206</v>
+      </c>
+      <c r="B85" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>206</v>
+      </c>
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>206</v>
+      </c>
+      <c r="B87" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>206</v>
+      </c>
+      <c r="B89" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <autoFilter ref="A1:C1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,17 +2602,59 @@
         <v>65</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>148</v>
+      </c>
+      <c r="D41" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>151</v>
+      </c>
+      <c r="D43" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E27"/>
+  <autoFilter ref="A1:E27" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3559,7 +4357,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Merged PR 3379: 31936 Updating configs to combine QA0 with QA1
Updated Icon DB reference to new QA1 Icon Db
Updated KitBuilder WebApi to point to new Mammoth QA URL

Related work items: #31936
</commit_message>
<xml_diff>
--- a/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
+++ b/DevOps/Server Setup/Security/Server Security Setup Input Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpesh.patel\source\repos\SCAD\DevOps\Server Setup\Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B88C8EBA-2D50-40B5-9E53-05AB4DF9199C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F3A8D10-BD75-46CA-B601-9DEA000D9A51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server List" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="215">
   <si>
     <t>WFM\Icon.Deploy.NonProd</t>
   </si>
@@ -655,6 +655,30 @@
   </si>
   <si>
     <t>PROD</t>
+  </si>
+  <si>
+    <t>WFM\IRMA.Deploy.Prod</t>
+  </si>
+  <si>
+    <t>WFM\Icon.Deploy.Prod</t>
+  </si>
+  <si>
+    <t>WFM\Mammoth.Deploy.Prod</t>
+  </si>
+  <si>
+    <t>wfm\IconInterfaceUserPrd</t>
+  </si>
+  <si>
+    <t>wfm\MammothPrd</t>
+  </si>
+  <si>
+    <t>WFM\NutriconService</t>
+  </si>
+  <si>
+    <t>wfm\IconWebPrd</t>
+  </si>
+  <si>
+    <t>WFM\SPOReports</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:A89"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2022,14 +2046,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" customWidth="1"/>
     <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
@@ -2642,6 +2667,188 @@
       </c>
       <c r="D43" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>212</v>
+      </c>
+      <c r="D50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>211</v>
+      </c>
+      <c r="D52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>213</v>
+      </c>
+      <c r="D53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>212</v>
+      </c>
+      <c r="D54" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>214</v>
+      </c>
+      <c r="D55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>